<commit_message>
Tightened up date codec definition and implementation Tightened up int/float/long/double definitions and implementations Stubbed out a listCodec and came up with some questions to consider Started documenting identifier types, though it will need to move to spec/
</commit_message>
<xml_diff>
--- a/types.xlsx
+++ b/types.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mbishop/Sides/Identifiers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mbishop/Sides/Identifiers/identifiers-js/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -473,7 +473,7 @@
   <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Removed double type and re-task float as a 64-bit decimal value float-32 is not very precise and internally is often just a float-64. Couldn't think of an identifier that wanted less decimal precision.
</commit_message>
<xml_diff>
--- a/types.xlsx
+++ b/types.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>struct</t>
   </si>
@@ -83,12 +83,6 @@
     <t>geo</t>
   </si>
   <si>
-    <t>an integer?</t>
-  </si>
-  <si>
-    <t>double</t>
-  </si>
-  <si>
     <t>EXT</t>
   </si>
   <si>
@@ -101,7 +95,7 @@
     <t>[long]</t>
   </si>
   <si>
-    <t>[double]</t>
+    <t>[float]</t>
   </si>
 </sst>
 </file>
@@ -473,7 +467,7 @@
   <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -481,7 +475,7 @@
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="5"/>
       <c r="B1" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -493,7 +487,7 @@
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
@@ -810,7 +804,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1">
         <v>0</v>
@@ -1006,7 +1000,7 @@
         <v>35</v>
       </c>
       <c r="K15" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
@@ -1050,7 +1044,7 @@
         <v>67</v>
       </c>
       <c r="K16" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
@@ -1098,7 +1092,7 @@
         <v>109</v>
       </c>
       <c r="K17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
@@ -1124,7 +1118,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" s="1">
         <v>1</v>
@@ -1143,10 +1137,10 @@
       </c>
       <c r="J18">
         <f>(B18*B3)+(C18*C3)+(D18*D3)+(E18*E3)+(F18*F3)+(G18*G3)+(H18*H3)+(I18*I3)</f>
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="K18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
@@ -1233,7 +1227,7 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>

</xml_diff>

<commit_message>
Fix tests for list codec Moved finder to a registration model Updated deps
</commit_message>
<xml_diff>
--- a/types.xlsx
+++ b/types.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>struct</t>
   </si>
@@ -74,12 +74,6 @@
     <t>any</t>
   </si>
   <si>
-    <t>ipv4</t>
-  </si>
-  <si>
-    <t>ipv6</t>
-  </si>
-  <si>
     <t>geo</t>
   </si>
   <si>
@@ -90,9 +84,6 @@
   </si>
   <si>
     <t>Byte 2</t>
-  </si>
-  <si>
-    <t>[long]</t>
   </si>
   <si>
     <t>[float]</t>
@@ -466,8 +457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -475,7 +466,7 @@
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="5"/>
       <c r="B1" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -487,7 +478,7 @@
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
@@ -979,10 +970,10 @@
         <v>1</v>
       </c>
       <c r="C15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -997,7 +988,7 @@
       </c>
       <c r="J15">
         <f>(B15*B3)+(C15*C3)+(D15*D3)+(E15*E3)+(F15*F3)+(G15*G3)+(H15*H3)+(I15*I3)</f>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="K15" t="s">
         <v>4</v>
@@ -1020,7 +1011,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
@@ -1028,8 +1019,12 @@
       <c r="D16" s="1">
         <v>0</v>
       </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
       <c r="G16" s="1">
         <v>0</v>
       </c>
@@ -1041,10 +1036,10 @@
       </c>
       <c r="J16">
         <f>(B16*B3)+(C16*C3)+(D16*D3)+(E16*E3)+(F16*F3)+(G16*G3)+(H16*H3)+(I16*I3)</f>
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="K16" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
@@ -1061,23 +1056,13 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1">
-        <v>1</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0</v>
-      </c>
-      <c r="D17" s="1">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1">
-        <v>1</v>
-      </c>
-      <c r="F17" s="1">
-        <v>0</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
       <c r="G17" s="1">
         <v>1</v>
       </c>
@@ -1089,10 +1074,7 @@
       </c>
       <c r="J17">
         <f>(B17*B3)+(C17*C3)+(D17*D3)+(E17*E3)+(F17*F3)+(G17*G3)+(H17*H3)+(I17*I3)</f>
-        <v>109</v>
-      </c>
-      <c r="K17" t="s">
-        <v>21</v>
+        <v>96</v>
       </c>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
@@ -1109,23 +1091,13 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1">
-        <v>0</v>
-      </c>
-      <c r="C18" s="1">
-        <v>1</v>
-      </c>
-      <c r="D18" s="1">
-        <v>0</v>
-      </c>
-      <c r="E18" s="1">
-        <v>1</v>
-      </c>
-      <c r="F18" s="1">
-        <v>0</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
       <c r="G18" s="1">
         <v>0</v>
       </c>
@@ -1137,10 +1109,7 @@
       </c>
       <c r="J18">
         <f>(B18*B3)+(C18*C3)+(D18*D3)+(E18*E3)+(F18*F3)+(G18*G3)+(H18*H3)+(I18*I3)</f>
-        <v>138</v>
-      </c>
-      <c r="K18" t="s">
-        <v>22</v>
+        <v>128</v>
       </c>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
@@ -1227,7 +1196,7 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>

</xml_diff>